<commit_message>
reverted commits due to homepage not working
</commit_message>
<xml_diff>
--- a/Introduction-to-Data/L3-and-L4:Spreadsheets-1&2/Misc/extract-text.xlsx
+++ b/Introduction-to-Data/L3-and-L4:Spreadsheets-1&2/Misc/extract-text.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marksoro/git-projects/Business-Analytics/Introduction-to-Data/L3-and-L4:Spreadsheets-1&amp;2/Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9C8DD5-CC35-654F-89D9-4A7FB1A2227F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C99216-1FD9-4F48-B9EF-918E379F54F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="2120" windowWidth="20960" windowHeight="18040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,21 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Sentence</t>
   </si>
@@ -64,6 +73,7 @@
         <sz val="12"/>
         <color rgb="FF6A6A6A"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>data practice</t>
     </r>
@@ -72,6 +82,7 @@
         <sz val="12"/>
         <color rgb="FF545454"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> we investigate the areas that experts predict will be the most fruitful. </t>
     </r>
@@ -132,6 +143,15 @@
   </si>
   <si>
     <t>- Sherlock Holmes</t>
+  </si>
+  <si>
+    <t>=UPPER(A1)</t>
+  </si>
+  <si>
+    <t>=PROPER(A1)</t>
+  </si>
+  <si>
+    <t>=LOWER(A1)</t>
   </si>
 </sst>
 </file>
@@ -150,11 +170,13 @@
       <sz val="12"/>
       <color rgb="FF545454"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF6A6A6A"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -215,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -299,12 +321,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -332,6 +369,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -945,16 +983,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B123ACF5-8B57-1541-8F86-0B27B7FE90CC}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="72.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.25">
@@ -966,7 +1004,7 @@
         <v xml:space="preserve">"IT IS A CAPITAL MISTAKE TO THEORIZE BEFORE ONE HAS DATA"  </v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>27</v>
       </c>
@@ -975,16 +1013,32 @@
         <v>- SHERLOCK HOLMES</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B4" t="str">
+    <row r="3" spans="1:2" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
         <f>PROPER(A1)</f>
         <v xml:space="preserve">"It Is A Capital Mistake To Theorize Before One Has Data"  </v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6" t="str">
+    <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="str">
         <f>LOWER(A1)</f>
         <v xml:space="preserve">"it is a capital mistake to theorize before one has data"  </v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>